<commit_message>
Updated Indonesia files compatible with v3.3.1
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
     <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -45,9 +50,6 @@
     <t>Source Data in 2007 dollars/metric ton CO2</t>
   </si>
   <si>
-    <t>Social Cost of Carbon ($)</t>
-  </si>
-  <si>
     <t>Data in 2012 dollars/gram CO2</t>
   </si>
   <si>
@@ -55,9 +57,6 @@
   </si>
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>When considering the Social Cost of Carbon, the U.S. government typically uses the figures based on</t>
   </si>
   <si>
     <t>a 3% discount rate, so this is the rate we use in this model.</t>
@@ -80,11 +79,20 @@
   <si>
     <t>https://www.whitehouse.gov/sites/default/files/omb/inforeg/scc-tsd-final-july-2015.pdf</t>
   </si>
+  <si>
+    <t>Social Cost of Carbon ($/g CO2e)</t>
+  </si>
+  <si>
+    <t>When considering the Social Cost of Carbon, meant to capture the long-term economic damage caused by one</t>
+  </si>
+  <si>
+    <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -266,6 +274,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -313,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,9 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -568,7 +581,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -591,52 +604,57 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
         <v>1.109</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>17</v>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +684,7 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="G1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -758,19 +776,19 @@
         <v>2010</v>
       </c>
       <c r="H4" s="12">
-        <f>B4*(About!$A$16)/10^6</f>
+        <f>B4*(About!$A$17)/10^6</f>
         <v>1.1090000000000001E-5</v>
       </c>
       <c r="I4" s="12">
-        <f>C4*(About!$A$16)/10^6</f>
+        <f>C4*(About!$A$17)/10^6</f>
         <v>3.4378999999999997E-5</v>
       </c>
       <c r="J4" s="12">
-        <f>D4*(About!$A$16)/10^6</f>
+        <f>D4*(About!$A$17)/10^6</f>
         <v>5.5450000000000006E-5</v>
       </c>
       <c r="K4" s="12">
-        <f>E4*(About!$A$16)/10^6</f>
+        <f>E4*(About!$A$17)/10^6</f>
         <v>9.5373999999999999E-5</v>
       </c>
     </row>
@@ -795,19 +813,19 @@
         <v>2011</v>
       </c>
       <c r="H5" s="12">
-        <f>B5*(About!$A$16)/10^6</f>
+        <f>B5*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I5" s="12">
-        <f>C5*(About!$A$16)/10^6</f>
+        <f>C5*(About!$A$17)/10^6</f>
         <v>3.5487999999999996E-5</v>
       </c>
       <c r="J5" s="12">
-        <f>D5*(About!$A$16)/10^6</f>
+        <f>D5*(About!$A$17)/10^6</f>
         <v>5.6558999999999998E-5</v>
       </c>
       <c r="K5" s="12">
-        <f>E5*(About!$A$16)/10^6</f>
+        <f>E5*(About!$A$17)/10^6</f>
         <v>9.9810000000000008E-5</v>
       </c>
     </row>
@@ -832,19 +850,19 @@
         <v>2012</v>
       </c>
       <c r="H6" s="12">
-        <f>B6*(About!$A$16)/10^6</f>
+        <f>B6*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I6" s="12">
-        <f>C6*(About!$A$16)/10^6</f>
+        <f>C6*(About!$A$17)/10^6</f>
         <v>3.6597000000000002E-5</v>
       </c>
       <c r="J6" s="12">
-        <f>D6*(About!$A$16)/10^6</f>
+        <f>D6*(About!$A$17)/10^6</f>
         <v>5.8777000000000003E-5</v>
       </c>
       <c r="K6" s="12">
-        <f>E6*(About!$A$16)/10^6</f>
+        <f>E6*(About!$A$17)/10^6</f>
         <v>1.03137E-4</v>
       </c>
     </row>
@@ -869,19 +887,19 @@
         <v>2013</v>
       </c>
       <c r="H7" s="12">
-        <f>B7*(About!$A$16)/10^6</f>
+        <f>B7*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I7" s="12">
-        <f>C7*(About!$A$16)/10^6</f>
+        <f>C7*(About!$A$17)/10^6</f>
         <v>3.7706000000000001E-5</v>
       </c>
       <c r="J7" s="12">
-        <f>D7*(About!$A$16)/10^6</f>
+        <f>D7*(About!$A$17)/10^6</f>
         <v>5.9885999999999995E-5</v>
       </c>
       <c r="K7" s="12">
-        <f>E7*(About!$A$16)/10^6</f>
+        <f>E7*(About!$A$17)/10^6</f>
         <v>1.0757299999999999E-4</v>
       </c>
     </row>
@@ -906,19 +924,19 @@
         <v>2014</v>
       </c>
       <c r="H8" s="12">
-        <f>B8*(About!$A$16)/10^6</f>
+        <f>B8*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I8" s="12">
-        <f>C8*(About!$A$16)/10^6</f>
+        <f>C8*(About!$A$17)/10^6</f>
         <v>3.8815E-5</v>
       </c>
       <c r="J8" s="12">
-        <f>D8*(About!$A$16)/10^6</f>
+        <f>D8*(About!$A$17)/10^6</f>
         <v>6.0994999999999995E-5</v>
       </c>
       <c r="K8" s="12">
-        <f>E8*(About!$A$16)/10^6</f>
+        <f>E8*(About!$A$17)/10^6</f>
         <v>1.12009E-4</v>
       </c>
     </row>
@@ -943,19 +961,19 @@
         <v>2015</v>
       </c>
       <c r="H9" s="12">
-        <f>B9*(About!$A$16)/10^6</f>
+        <f>B9*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I9" s="12">
-        <f>C9*(About!$A$16)/10^6</f>
+        <f>C9*(About!$A$17)/10^6</f>
         <v>3.9923999999999999E-5</v>
       </c>
       <c r="J9" s="12">
-        <f>D9*(About!$A$16)/10^6</f>
+        <f>D9*(About!$A$17)/10^6</f>
         <v>6.2104E-5</v>
       </c>
       <c r="K9" s="12">
-        <f>E9*(About!$A$16)/10^6</f>
+        <f>E9*(About!$A$17)/10^6</f>
         <v>1.1644499999999999E-4</v>
       </c>
     </row>
@@ -980,19 +998,19 @@
         <v>2016</v>
       </c>
       <c r="H10" s="12">
-        <f>B10*(About!$A$16)/10^6</f>
+        <f>B10*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I10" s="12">
-        <f>C10*(About!$A$16)/10^6</f>
+        <f>C10*(About!$A$17)/10^6</f>
         <v>4.2141999999999997E-5</v>
       </c>
       <c r="J10" s="12">
-        <f>D10*(About!$A$16)/10^6</f>
+        <f>D10*(About!$A$17)/10^6</f>
         <v>6.3213000000000006E-5</v>
       </c>
       <c r="K10" s="12">
-        <f>E10*(About!$A$16)/10^6</f>
+        <f>E10*(About!$A$17)/10^6</f>
         <v>1.1977199999999999E-4</v>
       </c>
     </row>
@@ -1017,19 +1035,19 @@
         <v>2017</v>
       </c>
       <c r="H11" s="12">
-        <f>B11*(About!$A$16)/10^6</f>
+        <f>B11*(About!$A$17)/10^6</f>
         <v>1.2199E-5</v>
       </c>
       <c r="I11" s="12">
-        <f>C11*(About!$A$16)/10^6</f>
+        <f>C11*(About!$A$17)/10^6</f>
         <v>4.3250999999999996E-5</v>
       </c>
       <c r="J11" s="12">
-        <f>D11*(About!$A$16)/10^6</f>
+        <f>D11*(About!$A$17)/10^6</f>
         <v>6.5430999999999991E-5</v>
       </c>
       <c r="K11" s="12">
-        <f>E11*(About!$A$16)/10^6</f>
+        <f>E11*(About!$A$17)/10^6</f>
         <v>1.24208E-4</v>
       </c>
     </row>
@@ -1054,19 +1072,19 @@
         <v>2018</v>
       </c>
       <c r="H12" s="12">
-        <f>B12*(About!$A$16)/10^6</f>
+        <f>B12*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I12" s="12">
-        <f>C12*(About!$A$16)/10^6</f>
+        <f>C12*(About!$A$17)/10^6</f>
         <v>4.4360000000000002E-5</v>
       </c>
       <c r="J12" s="12">
-        <f>D12*(About!$A$16)/10^6</f>
+        <f>D12*(About!$A$17)/10^6</f>
         <v>6.6539999999999997E-5</v>
       </c>
       <c r="K12" s="12">
-        <f>E12*(About!$A$16)/10^6</f>
+        <f>E12*(About!$A$17)/10^6</f>
         <v>1.28644E-4</v>
       </c>
     </row>
@@ -1091,19 +1109,19 @@
         <v>2019</v>
       </c>
       <c r="H13" s="12">
-        <f>B13*(About!$A$16)/10^6</f>
+        <f>B13*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I13" s="12">
-        <f>C13*(About!$A$16)/10^6</f>
+        <f>C13*(About!$A$17)/10^6</f>
         <v>4.5469000000000001E-5</v>
       </c>
       <c r="J13" s="12">
-        <f>D13*(About!$A$16)/10^6</f>
+        <f>D13*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="K13" s="12">
-        <f>E13*(About!$A$16)/10^6</f>
+        <f>E13*(About!$A$17)/10^6</f>
         <v>1.3307999999999999E-4</v>
       </c>
     </row>
@@ -1128,19 +1146,19 @@
         <v>2020</v>
       </c>
       <c r="H14" s="12">
-        <f>B14*(About!$A$16)/10^6</f>
+        <f>B14*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I14" s="12">
-        <f>C14*(About!$A$16)/10^6</f>
+        <f>C14*(About!$A$17)/10^6</f>
         <v>4.6578E-5</v>
       </c>
       <c r="J14" s="12">
-        <f>D14*(About!$A$16)/10^6</f>
+        <f>D14*(About!$A$17)/10^6</f>
         <v>6.8757999999999995E-5</v>
       </c>
       <c r="K14" s="12">
-        <f>E14*(About!$A$16)/10^6</f>
+        <f>E14*(About!$A$17)/10^6</f>
         <v>1.3640700000000001E-4</v>
       </c>
     </row>
@@ -1165,19 +1183,19 @@
         <v>2021</v>
       </c>
       <c r="H15" s="12">
-        <f>B15*(About!$A$16)/10^6</f>
+        <f>B15*(About!$A$17)/10^6</f>
         <v>1.3308E-5</v>
       </c>
       <c r="I15" s="12">
-        <f>C15*(About!$A$16)/10^6</f>
+        <f>C15*(About!$A$17)/10^6</f>
         <v>4.6578E-5</v>
       </c>
       <c r="J15" s="12">
-        <f>D15*(About!$A$16)/10^6</f>
+        <f>D15*(About!$A$17)/10^6</f>
         <v>6.9867E-5</v>
       </c>
       <c r="K15" s="12">
-        <f>E15*(About!$A$16)/10^6</f>
+        <f>E15*(About!$A$17)/10^6</f>
         <v>1.39734E-4</v>
       </c>
     </row>
@@ -1202,19 +1220,19 @@
         <v>2022</v>
       </c>
       <c r="H16" s="12">
-        <f>B16*(About!$A$16)/10^6</f>
+        <f>B16*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I16" s="12">
-        <f>C16*(About!$A$16)/10^6</f>
+        <f>C16*(About!$A$17)/10^6</f>
         <v>4.7686999999999999E-5</v>
       </c>
       <c r="J16" s="12">
-        <f>D16*(About!$A$16)/10^6</f>
+        <f>D16*(About!$A$17)/10^6</f>
         <v>7.0975999999999993E-5</v>
       </c>
       <c r="K16" s="12">
-        <f>E16*(About!$A$16)/10^6</f>
+        <f>E16*(About!$A$17)/10^6</f>
         <v>1.4306100000000002E-4</v>
       </c>
     </row>
@@ -1239,19 +1257,19 @@
         <v>2023</v>
       </c>
       <c r="H17" s="12">
-        <f>B17*(About!$A$16)/10^6</f>
+        <f>B17*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I17" s="12">
-        <f>C17*(About!$A$16)/10^6</f>
+        <f>C17*(About!$A$17)/10^6</f>
         <v>4.8795999999999998E-5</v>
       </c>
       <c r="J17" s="12">
-        <f>D17*(About!$A$16)/10^6</f>
+        <f>D17*(About!$A$17)/10^6</f>
         <v>7.2084999999999998E-5</v>
       </c>
       <c r="K17" s="12">
-        <f>E17*(About!$A$16)/10^6</f>
+        <f>E17*(About!$A$17)/10^6</f>
         <v>1.4638800000000001E-4</v>
       </c>
     </row>
@@ -1276,19 +1294,19 @@
         <v>2024</v>
       </c>
       <c r="H18" s="12">
-        <f>B18*(About!$A$16)/10^6</f>
+        <f>B18*(About!$A$17)/10^6</f>
         <v>1.4416999999999999E-5</v>
       </c>
       <c r="I18" s="12">
-        <f>C18*(About!$A$16)/10^6</f>
+        <f>C18*(About!$A$17)/10^6</f>
         <v>4.9905000000000004E-5</v>
       </c>
       <c r="J18" s="12">
-        <f>D18*(About!$A$16)/10^6</f>
+        <f>D18*(About!$A$17)/10^6</f>
         <v>7.3194000000000004E-5</v>
       </c>
       <c r="K18" s="12">
-        <f>E18*(About!$A$16)/10^6</f>
+        <f>E18*(About!$A$17)/10^6</f>
         <v>1.49715E-4</v>
       </c>
     </row>
@@ -1313,19 +1331,19 @@
         <v>2025</v>
       </c>
       <c r="H19" s="12">
-        <f>B19*(About!$A$16)/10^6</f>
+        <f>B19*(About!$A$17)/10^6</f>
         <v>1.5526E-5</v>
       </c>
       <c r="I19" s="12">
-        <f>C19*(About!$A$16)/10^6</f>
+        <f>C19*(About!$A$17)/10^6</f>
         <v>5.1013999999999996E-5</v>
       </c>
       <c r="J19" s="12">
-        <f>D19*(About!$A$16)/10^6</f>
+        <f>D19*(About!$A$17)/10^6</f>
         <v>7.5412000000000002E-5</v>
       </c>
       <c r="K19" s="12">
-        <f>E19*(About!$A$16)/10^6</f>
+        <f>E19*(About!$A$17)/10^6</f>
         <v>1.5304199999999999E-4</v>
       </c>
     </row>
@@ -1350,19 +1368,19 @@
         <v>2026</v>
       </c>
       <c r="H20" s="12">
-        <f>B20*(About!$A$16)/10^6</f>
+        <f>B20*(About!$A$17)/10^6</f>
         <v>1.5526E-5</v>
       </c>
       <c r="I20" s="12">
-        <f>C20*(About!$A$16)/10^6</f>
+        <f>C20*(About!$A$17)/10^6</f>
         <v>5.2122999999999995E-5</v>
       </c>
       <c r="J20" s="12">
-        <f>D20*(About!$A$16)/10^6</f>
+        <f>D20*(About!$A$17)/10^6</f>
         <v>7.6520999999999995E-5</v>
       </c>
       <c r="K20" s="12">
-        <f>E20*(About!$A$16)/10^6</f>
+        <f>E20*(About!$A$17)/10^6</f>
         <v>1.5636900000000001E-4</v>
       </c>
     </row>
@@ -1387,19 +1405,19 @@
         <v>2027</v>
       </c>
       <c r="H21" s="12">
-        <f>B21*(About!$A$16)/10^6</f>
+        <f>B21*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I21" s="12">
-        <f>C21*(About!$A$16)/10^6</f>
+        <f>C21*(About!$A$17)/10^6</f>
         <v>5.3232000000000001E-5</v>
       </c>
       <c r="J21" s="12">
-        <f>D21*(About!$A$16)/10^6</f>
+        <f>D21*(About!$A$17)/10^6</f>
         <v>7.763E-5</v>
       </c>
       <c r="K21" s="12">
-        <f>E21*(About!$A$16)/10^6</f>
+        <f>E21*(About!$A$17)/10^6</f>
         <v>1.5858699999999999E-4</v>
       </c>
     </row>
@@ -1424,19 +1442,19 @@
         <v>2028</v>
       </c>
       <c r="H22" s="12">
-        <f>B22*(About!$A$16)/10^6</f>
+        <f>B22*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I22" s="12">
-        <f>C22*(About!$A$16)/10^6</f>
+        <f>C22*(About!$A$17)/10^6</f>
         <v>5.4341E-5</v>
       </c>
       <c r="J22" s="12">
-        <f>D22*(About!$A$16)/10^6</f>
+        <f>D22*(About!$A$17)/10^6</f>
         <v>7.8739000000000006E-5</v>
       </c>
       <c r="K22" s="12">
-        <f>E22*(About!$A$16)/10^6</f>
+        <f>E22*(About!$A$17)/10^6</f>
         <v>1.6191399999999998E-4</v>
       </c>
     </row>
@@ -1461,19 +1479,19 @@
         <v>2029</v>
       </c>
       <c r="H23" s="12">
-        <f>B23*(About!$A$16)/10^6</f>
+        <f>B23*(About!$A$17)/10^6</f>
         <v>1.6634999999999999E-5</v>
       </c>
       <c r="I23" s="12">
-        <f>C23*(About!$A$16)/10^6</f>
+        <f>C23*(About!$A$17)/10^6</f>
         <v>5.4341E-5</v>
       </c>
       <c r="J23" s="12">
-        <f>D23*(About!$A$16)/10^6</f>
+        <f>D23*(About!$A$17)/10^6</f>
         <v>7.9847999999999999E-5</v>
       </c>
       <c r="K23" s="12">
-        <f>E23*(About!$A$16)/10^6</f>
+        <f>E23*(About!$A$17)/10^6</f>
         <v>1.65241E-4</v>
       </c>
     </row>
@@ -1498,19 +1516,19 @@
         <v>2030</v>
       </c>
       <c r="H24" s="12">
-        <f>B24*(About!$A$16)/10^6</f>
+        <f>B24*(About!$A$17)/10^6</f>
         <v>1.7743999999999998E-5</v>
       </c>
       <c r="I24" s="12">
-        <f>C24*(About!$A$16)/10^6</f>
+        <f>C24*(About!$A$17)/10^6</f>
         <v>5.5450000000000006E-5</v>
       </c>
       <c r="J24" s="12">
-        <f>D24*(About!$A$16)/10^6</f>
+        <f>D24*(About!$A$17)/10^6</f>
         <v>8.0956999999999991E-5</v>
       </c>
       <c r="K24" s="12">
-        <f>E24*(About!$A$16)/10^6</f>
+        <f>E24*(About!$A$17)/10^6</f>
         <v>1.6856799999999999E-4</v>
       </c>
     </row>
@@ -1535,19 +1553,19 @@
         <v>2031</v>
       </c>
       <c r="H25" s="12">
-        <f>B25*(About!$A$16)/10^6</f>
+        <f>B25*(About!$A$17)/10^6</f>
         <v>1.7743999999999998E-5</v>
       </c>
       <c r="I25" s="12">
-        <f>C25*(About!$A$16)/10^6</f>
+        <f>C25*(About!$A$17)/10^6</f>
         <v>5.6558999999999998E-5</v>
       </c>
       <c r="J25" s="12">
-        <f>D25*(About!$A$16)/10^6</f>
+        <f>D25*(About!$A$17)/10^6</f>
         <v>8.2065999999999997E-5</v>
       </c>
       <c r="K25" s="12">
-        <f>E25*(About!$A$16)/10^6</f>
+        <f>E25*(About!$A$17)/10^6</f>
         <v>1.7189500000000001E-4</v>
       </c>
     </row>
@@ -1572,19 +1590,19 @@
         <v>2032</v>
       </c>
       <c r="H26" s="12">
-        <f>B26*(About!$A$16)/10^6</f>
+        <f>B26*(About!$A$17)/10^6</f>
         <v>1.8853000000000001E-5</v>
       </c>
       <c r="I26" s="12">
-        <f>C26*(About!$A$16)/10^6</f>
+        <f>C26*(About!$A$17)/10^6</f>
         <v>5.7667999999999997E-5</v>
       </c>
       <c r="J26" s="12">
-        <f>D26*(About!$A$16)/10^6</f>
+        <f>D26*(About!$A$17)/10^6</f>
         <v>8.3175000000000002E-5</v>
       </c>
       <c r="K26" s="12">
-        <f>E26*(About!$A$16)/10^6</f>
+        <f>E26*(About!$A$17)/10^6</f>
         <v>1.75222E-4</v>
       </c>
     </row>
@@ -1609,19 +1627,19 @@
         <v>2033</v>
       </c>
       <c r="H27" s="12">
-        <f>B27*(About!$A$16)/10^6</f>
+        <f>B27*(About!$A$17)/10^6</f>
         <v>1.8853000000000001E-5</v>
       </c>
       <c r="I27" s="12">
-        <f>C27*(About!$A$16)/10^6</f>
+        <f>C27*(About!$A$17)/10^6</f>
         <v>5.8777000000000003E-5</v>
       </c>
       <c r="J27" s="12">
-        <f>D27*(About!$A$16)/10^6</f>
+        <f>D27*(About!$A$17)/10^6</f>
         <v>8.4283999999999995E-5</v>
       </c>
       <c r="K27" s="12">
-        <f>E27*(About!$A$16)/10^6</f>
+        <f>E27*(About!$A$17)/10^6</f>
         <v>1.7854900000000001E-4</v>
       </c>
     </row>
@@ -1646,19 +1664,19 @@
         <v>2034</v>
       </c>
       <c r="H28" s="12">
-        <f>B28*(About!$A$16)/10^6</f>
+        <f>B28*(About!$A$17)/10^6</f>
         <v>1.9962E-5</v>
       </c>
       <c r="I28" s="12">
-        <f>C28*(About!$A$16)/10^6</f>
+        <f>C28*(About!$A$17)/10^6</f>
         <v>5.9885999999999995E-5</v>
       </c>
       <c r="J28" s="12">
-        <f>D28*(About!$A$16)/10^6</f>
+        <f>D28*(About!$A$17)/10^6</f>
         <v>8.5393E-5</v>
       </c>
       <c r="K28" s="12">
-        <f>E28*(About!$A$16)/10^6</f>
+        <f>E28*(About!$A$17)/10^6</f>
         <v>1.81876E-4</v>
       </c>
     </row>
@@ -1683,19 +1701,19 @@
         <v>2035</v>
       </c>
       <c r="H29" s="12">
-        <f>B29*(About!$A$16)/10^6</f>
+        <f>B29*(About!$A$17)/10^6</f>
         <v>1.9962E-5</v>
       </c>
       <c r="I29" s="12">
-        <f>C29*(About!$A$16)/10^6</f>
+        <f>C29*(About!$A$17)/10^6</f>
         <v>6.0994999999999995E-5</v>
       </c>
       <c r="J29" s="12">
-        <f>D29*(About!$A$16)/10^6</f>
+        <f>D29*(About!$A$17)/10^6</f>
         <v>8.6501999999999993E-5</v>
       </c>
       <c r="K29" s="12">
-        <f>E29*(About!$A$16)/10^6</f>
+        <f>E29*(About!$A$17)/10^6</f>
         <v>1.86312E-4</v>
       </c>
     </row>
@@ -1720,19 +1738,19 @@
         <v>2036</v>
       </c>
       <c r="H30" s="12">
-        <f>B30*(About!$A$16)/10^6</f>
+        <f>B30*(About!$A$17)/10^6</f>
         <v>2.1070999999999999E-5</v>
       </c>
       <c r="I30" s="12">
-        <f>C30*(About!$A$16)/10^6</f>
+        <f>C30*(About!$A$17)/10^6</f>
         <v>6.2104E-5</v>
       </c>
       <c r="J30" s="12">
-        <f>D30*(About!$A$16)/10^6</f>
+        <f>D30*(About!$A$17)/10^6</f>
         <v>8.7610999999999999E-5</v>
       </c>
       <c r="K30" s="12">
-        <f>E30*(About!$A$16)/10^6</f>
+        <f>E30*(About!$A$17)/10^6</f>
         <v>1.8963900000000002E-4</v>
       </c>
     </row>
@@ -1757,19 +1775,19 @@
         <v>2037</v>
       </c>
       <c r="H31" s="12">
-        <f>B31*(About!$A$16)/10^6</f>
+        <f>B31*(About!$A$17)/10^6</f>
         <v>2.1070999999999999E-5</v>
       </c>
       <c r="I31" s="12">
-        <f>C31*(About!$A$16)/10^6</f>
+        <f>C31*(About!$A$17)/10^6</f>
         <v>6.3213000000000006E-5</v>
       </c>
       <c r="J31" s="12">
-        <f>D31*(About!$A$16)/10^6</f>
+        <f>D31*(About!$A$17)/10^6</f>
         <v>8.9828999999999997E-5</v>
       </c>
       <c r="K31" s="12">
-        <f>E31*(About!$A$16)/10^6</f>
+        <f>E31*(About!$A$17)/10^6</f>
         <v>1.9296600000000001E-4</v>
       </c>
     </row>
@@ -1794,19 +1812,19 @@
         <v>2038</v>
       </c>
       <c r="H32" s="12">
-        <f>B32*(About!$A$16)/10^6</f>
+        <f>B32*(About!$A$17)/10^6</f>
         <v>2.2180000000000001E-5</v>
       </c>
       <c r="I32" s="12">
-        <f>C32*(About!$A$16)/10^6</f>
+        <f>C32*(About!$A$17)/10^6</f>
         <v>6.4321999999999998E-5</v>
       </c>
       <c r="J32" s="12">
-        <f>D32*(About!$A$16)/10^6</f>
+        <f>D32*(About!$A$17)/10^6</f>
         <v>9.0938000000000002E-5</v>
       </c>
       <c r="K32" s="12">
-        <f>E32*(About!$A$16)/10^6</f>
+        <f>E32*(About!$A$17)/10^6</f>
         <v>1.96293E-4</v>
       </c>
     </row>
@@ -1831,19 +1849,19 @@
         <v>2039</v>
       </c>
       <c r="H33" s="12">
-        <f>B33*(About!$A$16)/10^6</f>
+        <f>B33*(About!$A$17)/10^6</f>
         <v>2.2180000000000001E-5</v>
       </c>
       <c r="I33" s="12">
-        <f>C33*(About!$A$16)/10^6</f>
+        <f>C33*(About!$A$17)/10^6</f>
         <v>6.5430999999999991E-5</v>
       </c>
       <c r="J33" s="12">
-        <f>D33*(About!$A$16)/10^6</f>
+        <f>D33*(About!$A$17)/10^6</f>
         <v>9.2046999999999995E-5</v>
       </c>
       <c r="K33" s="12">
-        <f>E33*(About!$A$16)/10^6</f>
+        <f>E33*(About!$A$17)/10^6</f>
         <v>1.9962000000000002E-4</v>
       </c>
     </row>
@@ -1868,19 +1886,19 @@
         <v>2040</v>
       </c>
       <c r="H34" s="12">
-        <f>B34*(About!$A$16)/10^6</f>
+        <f>B34*(About!$A$17)/10^6</f>
         <v>2.3289E-5</v>
       </c>
       <c r="I34" s="12">
-        <f>C34*(About!$A$16)/10^6</f>
+        <f>C34*(About!$A$17)/10^6</f>
         <v>6.6539999999999997E-5</v>
       </c>
       <c r="J34" s="12">
-        <f>D34*(About!$A$16)/10^6</f>
+        <f>D34*(About!$A$17)/10^6</f>
         <v>9.3156000000000001E-5</v>
       </c>
       <c r="K34" s="12">
-        <f>E34*(About!$A$16)/10^6</f>
+        <f>E34*(About!$A$17)/10^6</f>
         <v>2.0294700000000001E-4</v>
       </c>
     </row>
@@ -1905,19 +1923,19 @@
         <v>2041</v>
       </c>
       <c r="H35" s="12">
-        <f>B35*(About!$A$16)/10^6</f>
+        <f>B35*(About!$A$17)/10^6</f>
         <v>2.3289E-5</v>
       </c>
       <c r="I35" s="12">
-        <f>C35*(About!$A$16)/10^6</f>
+        <f>C35*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="J35" s="12">
-        <f>D35*(About!$A$16)/10^6</f>
+        <f>D35*(About!$A$17)/10^6</f>
         <v>9.4265000000000006E-5</v>
       </c>
       <c r="K35" s="12">
-        <f>E35*(About!$A$16)/10^6</f>
+        <f>E35*(About!$A$17)/10^6</f>
         <v>2.06274E-4</v>
       </c>
     </row>
@@ -1942,19 +1960,19 @@
         <v>2042</v>
       </c>
       <c r="H36" s="12">
-        <f>B36*(About!$A$16)/10^6</f>
+        <f>B36*(About!$A$17)/10^6</f>
         <v>2.4397999999999999E-5</v>
       </c>
       <c r="I36" s="12">
-        <f>C36*(About!$A$16)/10^6</f>
+        <f>C36*(About!$A$17)/10^6</f>
         <v>6.7649000000000002E-5</v>
       </c>
       <c r="J36" s="12">
-        <f>D36*(About!$A$16)/10^6</f>
+        <f>D36*(About!$A$17)/10^6</f>
         <v>9.5373999999999999E-5</v>
       </c>
       <c r="K36" s="12">
-        <f>E36*(About!$A$16)/10^6</f>
+        <f>E36*(About!$A$17)/10^6</f>
         <v>2.0960099999999999E-4</v>
       </c>
     </row>
@@ -1979,19 +1997,19 @@
         <v>2043</v>
       </c>
       <c r="H37" s="12">
-        <f>B37*(About!$A$16)/10^6</f>
+        <f>B37*(About!$A$17)/10^6</f>
         <v>2.4397999999999999E-5</v>
       </c>
       <c r="I37" s="12">
-        <f>C37*(About!$A$16)/10^6</f>
+        <f>C37*(About!$A$17)/10^6</f>
         <v>6.8757999999999995E-5</v>
       </c>
       <c r="J37" s="12">
-        <f>D37*(About!$A$16)/10^6</f>
+        <f>D37*(About!$A$17)/10^6</f>
         <v>9.6483000000000004E-5</v>
       </c>
       <c r="K37" s="12">
-        <f>E37*(About!$A$16)/10^6</f>
+        <f>E37*(About!$A$17)/10^6</f>
         <v>2.1292800000000001E-4</v>
       </c>
     </row>
@@ -2016,19 +2034,19 @@
         <v>2044</v>
       </c>
       <c r="H38" s="12">
-        <f>B38*(About!$A$16)/10^6</f>
+        <f>B38*(About!$A$17)/10^6</f>
         <v>2.5506999999999998E-5</v>
       </c>
       <c r="I38" s="12">
-        <f>C38*(About!$A$16)/10^6</f>
+        <f>C38*(About!$A$17)/10^6</f>
         <v>6.9867E-5</v>
       </c>
       <c r="J38" s="12">
-        <f>D38*(About!$A$16)/10^6</f>
+        <f>D38*(About!$A$17)/10^6</f>
         <v>9.7591999999999997E-5</v>
       </c>
       <c r="K38" s="12">
-        <f>E38*(About!$A$16)/10^6</f>
+        <f>E38*(About!$A$17)/10^6</f>
         <v>2.1514599999999999E-4</v>
       </c>
     </row>
@@ -2053,19 +2071,19 @@
         <v>2045</v>
       </c>
       <c r="H39" s="12">
-        <f>B39*(About!$A$16)/10^6</f>
+        <f>B39*(About!$A$17)/10^6</f>
         <v>2.5506999999999998E-5</v>
       </c>
       <c r="I39" s="12">
-        <f>C39*(About!$A$16)/10^6</f>
+        <f>C39*(About!$A$17)/10^6</f>
         <v>7.0975999999999993E-5</v>
       </c>
       <c r="J39" s="12">
-        <f>D39*(About!$A$16)/10^6</f>
+        <f>D39*(About!$A$17)/10^6</f>
         <v>9.8700999999999989E-5</v>
       </c>
       <c r="K39" s="12">
-        <f>E39*(About!$A$16)/10^6</f>
+        <f>E39*(About!$A$17)/10^6</f>
         <v>2.1847299999999998E-4</v>
       </c>
     </row>
@@ -2090,19 +2108,19 @@
         <v>2046</v>
       </c>
       <c r="H40" s="12">
-        <f>B40*(About!$A$16)/10^6</f>
+        <f>B40*(About!$A$17)/10^6</f>
         <v>2.6616000000000001E-5</v>
       </c>
       <c r="I40" s="12">
-        <f>C40*(About!$A$16)/10^6</f>
+        <f>C40*(About!$A$17)/10^6</f>
         <v>7.2084999999999998E-5</v>
       </c>
       <c r="J40" s="12">
-        <f>D40*(About!$A$16)/10^6</f>
+        <f>D40*(About!$A$17)/10^6</f>
         <v>9.9810000000000008E-5</v>
       </c>
       <c r="K40" s="12">
-        <f>E40*(About!$A$16)/10^6</f>
+        <f>E40*(About!$A$17)/10^6</f>
         <v>2.2180000000000002E-4</v>
       </c>
     </row>
@@ -2127,19 +2145,19 @@
         <v>2047</v>
       </c>
       <c r="H41" s="12">
-        <f>B41*(About!$A$16)/10^6</f>
+        <f>B41*(About!$A$17)/10^6</f>
         <v>2.6616000000000001E-5</v>
       </c>
       <c r="I41" s="12">
-        <f>C41*(About!$A$16)/10^6</f>
+        <f>C41*(About!$A$17)/10^6</f>
         <v>7.3194000000000004E-5</v>
       </c>
       <c r="J41" s="12">
-        <f>D41*(About!$A$16)/10^6</f>
+        <f>D41*(About!$A$17)/10^6</f>
         <v>1.0202799999999999E-4</v>
       </c>
       <c r="K41" s="12">
-        <f>E41*(About!$A$16)/10^6</f>
+        <f>E41*(About!$A$17)/10^6</f>
         <v>2.2512700000000001E-4</v>
       </c>
     </row>
@@ -2164,19 +2182,19 @@
         <v>2048</v>
       </c>
       <c r="H42" s="12">
-        <f>B42*(About!$A$16)/10^6</f>
+        <f>B42*(About!$A$17)/10^6</f>
         <v>2.7725000000000003E-5</v>
       </c>
       <c r="I42" s="12">
-        <f>C42*(About!$A$16)/10^6</f>
+        <f>C42*(About!$A$17)/10^6</f>
         <v>7.4302999999999997E-5</v>
       </c>
       <c r="J42" s="12">
-        <f>D42*(About!$A$16)/10^6</f>
+        <f>D42*(About!$A$17)/10^6</f>
         <v>1.03137E-4</v>
       </c>
       <c r="K42" s="12">
-        <f>E42*(About!$A$16)/10^6</f>
+        <f>E42*(About!$A$17)/10^6</f>
         <v>2.2845400000000001E-4</v>
       </c>
     </row>
@@ -2201,19 +2219,19 @@
         <v>2049</v>
       </c>
       <c r="H43" s="12">
-        <f>B43*(About!$A$16)/10^6</f>
+        <f>B43*(About!$A$17)/10^6</f>
         <v>2.7725000000000003E-5</v>
       </c>
       <c r="I43" s="12">
-        <f>C43*(About!$A$16)/10^6</f>
+        <f>C43*(About!$A$17)/10^6</f>
         <v>7.5412000000000002E-5</v>
       </c>
       <c r="J43" s="12">
-        <f>D43*(About!$A$16)/10^6</f>
+        <f>D43*(About!$A$17)/10^6</f>
         <v>1.0424599999999999E-4</v>
       </c>
       <c r="K43" s="12">
-        <f>E43*(About!$A$16)/10^6</f>
+        <f>E43*(About!$A$17)/10^6</f>
         <v>2.31781E-4</v>
       </c>
     </row>
@@ -2238,19 +2256,19 @@
         <v>2050</v>
       </c>
       <c r="H44" s="12">
-        <f>B44*(About!$A$16)/10^6</f>
+        <f>B44*(About!$A$17)/10^6</f>
         <v>2.8833999999999999E-5</v>
       </c>
       <c r="I44" s="12">
-        <f>C44*(About!$A$16)/10^6</f>
+        <f>C44*(About!$A$17)/10^6</f>
         <v>7.6520999999999995E-5</v>
       </c>
       <c r="J44" s="12">
-        <f>D44*(About!$A$16)/10^6</f>
+        <f>D44*(About!$A$17)/10^6</f>
         <v>1.0535500000000001E-4</v>
       </c>
       <c r="K44" s="12">
-        <f>E44*(About!$A$16)/10^6</f>
+        <f>E44*(About!$A$17)/10^6</f>
         <v>2.3510800000000001E-4</v>
       </c>
     </row>
@@ -2266,7 +2284,9 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2278,7 +2298,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>